<commit_message>
2018-07-04 cohort 2 update
</commit_message>
<xml_diff>
--- a/Data/2018-07-01_HS_datasheet.xlsx
+++ b/Data/2018-07-01_HS_datasheet.xlsx
@@ -319,6 +319,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="yyyy\-mm\-dd"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -350,9 +353,9 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,13 +689,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I521"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="I81" sqref="I81"/>
+    <sheetView tabSelected="1" topLeftCell="B78" workbookViewId="0">
+      <selection activeCell="N94" sqref="N94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="6" max="6" width="11.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
@@ -711,7 +715,7 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
       <c r="G1" t="s">
@@ -720,7 +724,7 @@
       <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
     </row>
@@ -740,10 +744,10 @@
       <c r="E2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I2" s="1">
+      <c r="I2" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -763,10 +767,10 @@
       <c r="E3" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="I3" s="1">
+      <c r="I3" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -786,10 +790,10 @@
       <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I4" s="1">
+      <c r="I4" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -809,10 +813,10 @@
       <c r="E5" t="s">
         <v>11</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="I5" s="1">
+      <c r="I5" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -832,10 +836,10 @@
       <c r="E6" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="I6" s="1">
+      <c r="I6" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -855,10 +859,10 @@
       <c r="E7" t="s">
         <v>13</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="1">
+      <c r="I7" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -878,10 +882,10 @@
       <c r="E8" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I8" s="1">
+      <c r="I8" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -901,7 +905,7 @@
       <c r="E9" t="s">
         <v>11</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="F9" s="1" t="s">
         <v>35</v>
       </c>
       <c r="G9">
@@ -910,7 +914,7 @@
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="I9" s="1">
+      <c r="I9" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -930,13 +934,13 @@
       <c r="E10" t="s">
         <v>11</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="1" t="s">
         <v>36</v>
       </c>
       <c r="G10">
         <v>38.4</v>
       </c>
-      <c r="I10" s="1">
+      <c r="I10" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -956,10 +960,10 @@
       <c r="E11" t="s">
         <v>11</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="F11" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I11" s="1">
+      <c r="I11" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -979,10 +983,10 @@
       <c r="E12" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="F12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="1">
+      <c r="I12" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1002,10 +1006,10 @@
       <c r="E13" t="s">
         <v>11</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="F13" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="1">
+      <c r="I13" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1025,13 +1029,13 @@
       <c r="E14" t="s">
         <v>13</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="1" t="s">
         <v>40</v>
       </c>
       <c r="G14">
         <v>38.200000000000003</v>
       </c>
-      <c r="I14" s="1">
+      <c r="I14" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1054,7 +1058,7 @@
       <c r="H15">
         <v>0</v>
       </c>
-      <c r="I15" s="1">
+      <c r="I15" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1074,13 +1078,13 @@
       <c r="E16" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="F16" s="1" t="s">
         <v>67</v>
       </c>
       <c r="H16">
         <v>0</v>
       </c>
-      <c r="I16" s="1">
+      <c r="I16" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1103,7 +1107,7 @@
       <c r="H17">
         <v>0</v>
       </c>
-      <c r="I17" s="1">
+      <c r="I17" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1123,13 +1127,13 @@
       <c r="E18" t="s">
         <v>13</v>
       </c>
-      <c r="F18" s="2" t="s">
+      <c r="F18" s="1" t="s">
         <v>68</v>
       </c>
       <c r="H18">
         <v>0</v>
       </c>
-      <c r="I18" s="1">
+      <c r="I18" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1149,13 +1153,13 @@
       <c r="E19" t="s">
         <v>11</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="F19" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H19">
         <v>0</v>
       </c>
-      <c r="I19" s="1">
+      <c r="I19" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1178,7 +1182,7 @@
       <c r="H20">
         <v>0</v>
       </c>
-      <c r="I20" s="1">
+      <c r="I20" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1198,13 +1202,13 @@
       <c r="E21" t="s">
         <v>11</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="F21" s="1" t="s">
         <v>69</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
-      <c r="I21" s="1">
+      <c r="I21" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1227,7 +1231,7 @@
       <c r="H22">
         <v>0</v>
       </c>
-      <c r="I22" s="1">
+      <c r="I22" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1250,7 +1254,7 @@
       <c r="H23">
         <v>0</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1270,13 +1274,13 @@
       <c r="E24" t="s">
         <v>11</v>
       </c>
-      <c r="F24" s="2" t="s">
+      <c r="F24" s="1" t="s">
         <v>70</v>
       </c>
       <c r="H24">
         <v>0</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1299,7 +1303,7 @@
       <c r="H25">
         <v>0</v>
       </c>
-      <c r="I25" s="1">
+      <c r="I25" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1322,7 +1326,7 @@
       <c r="H26">
         <v>0</v>
       </c>
-      <c r="I26" s="1">
+      <c r="I26" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1342,13 +1346,13 @@
       <c r="E27" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="2" t="s">
+      <c r="F27" s="1" t="s">
         <v>71</v>
       </c>
       <c r="H27">
         <v>0</v>
       </c>
-      <c r="I27" s="1">
+      <c r="I27" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1368,13 +1372,13 @@
       <c r="E28" t="s">
         <v>11</v>
       </c>
-      <c r="F28" s="2" t="s">
+      <c r="F28" s="1" t="s">
         <v>41</v>
       </c>
       <c r="H28">
         <v>0</v>
       </c>
-      <c r="I28" s="1">
+      <c r="I28" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1394,13 +1398,13 @@
       <c r="E29" t="s">
         <v>13</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="1" t="s">
         <v>42</v>
       </c>
       <c r="H29">
         <v>0</v>
       </c>
-      <c r="I29" s="1">
+      <c r="I29" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1420,13 +1424,13 @@
       <c r="E30" t="s">
         <v>11</v>
       </c>
-      <c r="F30" s="2" t="s">
+      <c r="F30" s="1" t="s">
         <v>43</v>
       </c>
       <c r="H30">
         <v>0</v>
       </c>
-      <c r="I30" s="1">
+      <c r="I30" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1446,13 +1450,13 @@
       <c r="E31" t="s">
         <v>13</v>
       </c>
-      <c r="F31" s="2" t="s">
+      <c r="F31" s="1" t="s">
         <v>44</v>
       </c>
       <c r="H31">
         <v>0</v>
       </c>
-      <c r="I31" s="1">
+      <c r="I31" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1472,13 +1476,13 @@
       <c r="E32" t="s">
         <v>13</v>
       </c>
-      <c r="F32" s="2" t="s">
+      <c r="F32" s="1" t="s">
         <v>45</v>
       </c>
       <c r="H32">
         <v>0</v>
       </c>
-      <c r="I32" s="1">
+      <c r="I32" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1498,13 +1502,13 @@
       <c r="E33" t="s">
         <v>13</v>
       </c>
-      <c r="F33" s="2" t="s">
+      <c r="F33" s="1" t="s">
         <v>46</v>
       </c>
       <c r="H33">
         <v>0</v>
       </c>
-      <c r="I33" s="1">
+      <c r="I33" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1524,10 +1528,10 @@
       <c r="E34" t="s">
         <v>11</v>
       </c>
-      <c r="F34" s="2" t="s">
+      <c r="F34" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="I34" s="1">
+      <c r="I34" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1547,13 +1551,13 @@
       <c r="E35" t="s">
         <v>13</v>
       </c>
-      <c r="F35" s="2" t="s">
+      <c r="F35" s="1" t="s">
         <v>48</v>
       </c>
       <c r="H35">
         <v>0</v>
       </c>
-      <c r="I35" s="1">
+      <c r="I35" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1573,10 +1577,10 @@
       <c r="E36" t="s">
         <v>11</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F36" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I36" s="1">
+      <c r="I36" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1596,10 +1600,10 @@
       <c r="E37" t="s">
         <v>11</v>
       </c>
-      <c r="F37" s="2" t="s">
+      <c r="F37" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I37" s="1">
+      <c r="I37" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1619,13 +1623,13 @@
       <c r="E38" t="s">
         <v>13</v>
       </c>
-      <c r="F38" s="2" t="s">
+      <c r="F38" s="1" t="s">
         <v>51</v>
       </c>
       <c r="H38">
         <v>0</v>
       </c>
-      <c r="I38" s="1">
+      <c r="I38" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1645,10 +1649,10 @@
       <c r="E39" t="s">
         <v>13</v>
       </c>
-      <c r="F39" s="2" t="s">
+      <c r="F39" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I39" s="1">
+      <c r="I39" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1668,13 +1672,13 @@
       <c r="E40" t="s">
         <v>13</v>
       </c>
-      <c r="F40" s="2" t="s">
+      <c r="F40" s="1" t="s">
         <v>53</v>
       </c>
       <c r="H40">
         <v>0</v>
       </c>
-      <c r="I40" s="1">
+      <c r="I40" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1694,13 +1698,13 @@
       <c r="E41" t="s">
         <v>11</v>
       </c>
-      <c r="F41" s="2" t="s">
+      <c r="F41" s="1" t="s">
         <v>54</v>
       </c>
       <c r="H41">
         <v>0</v>
       </c>
-      <c r="I41" s="1">
+      <c r="I41" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1720,7 +1724,7 @@
       <c r="E42" t="s">
         <v>13</v>
       </c>
-      <c r="F42" s="2" t="s">
+      <c r="F42" s="1" t="s">
         <v>55</v>
       </c>
       <c r="G42">
@@ -1729,7 +1733,7 @@
       <c r="H42">
         <v>0</v>
       </c>
-      <c r="I42" s="1">
+      <c r="I42" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1749,7 +1753,7 @@
       <c r="E43" t="s">
         <v>13</v>
       </c>
-      <c r="F43" s="2" t="s">
+      <c r="F43" s="1" t="s">
         <v>56</v>
       </c>
       <c r="G43">
@@ -1758,7 +1762,7 @@
       <c r="H43">
         <v>0</v>
       </c>
-      <c r="I43" s="1">
+      <c r="I43" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1778,7 +1782,7 @@
       <c r="E44" t="s">
         <v>13</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="F44" s="1" t="s">
         <v>57</v>
       </c>
       <c r="G44">
@@ -1787,7 +1791,7 @@
       <c r="H44">
         <v>0</v>
       </c>
-      <c r="I44" s="1">
+      <c r="I44" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1807,7 +1811,7 @@
       <c r="E45" t="s">
         <v>13</v>
       </c>
-      <c r="F45" s="2" t="s">
+      <c r="F45" s="1" t="s">
         <v>58</v>
       </c>
       <c r="G45">
@@ -1816,7 +1820,7 @@
       <c r="H45">
         <v>0</v>
       </c>
-      <c r="I45" s="1">
+      <c r="I45" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1836,7 +1840,7 @@
       <c r="E46" t="s">
         <v>11</v>
       </c>
-      <c r="F46" s="2" t="s">
+      <c r="F46" s="1" t="s">
         <v>59</v>
       </c>
       <c r="G46">
@@ -1845,7 +1849,7 @@
       <c r="H46">
         <v>0</v>
       </c>
-      <c r="I46" s="1">
+      <c r="I46" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1865,10 +1869,10 @@
       <c r="E47" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="2" t="s">
+      <c r="F47" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I47" s="1">
+      <c r="I47" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1888,7 +1892,7 @@
       <c r="E48" t="s">
         <v>11</v>
       </c>
-      <c r="F48" s="2" t="s">
+      <c r="F48" s="1" t="s">
         <v>61</v>
       </c>
       <c r="G48">
@@ -1897,7 +1901,7 @@
       <c r="H48">
         <v>0</v>
       </c>
-      <c r="I48" s="1">
+      <c r="I48" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1917,13 +1921,13 @@
       <c r="E49" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="2" t="s">
+      <c r="F49" s="1" t="s">
         <v>62</v>
       </c>
       <c r="H49">
         <v>0</v>
       </c>
-      <c r="I49" s="1">
+      <c r="I49" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1943,10 +1947,10 @@
       <c r="E50" t="s">
         <v>11</v>
       </c>
-      <c r="F50" s="2" t="s">
+      <c r="F50" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="I50" s="1">
+      <c r="I50" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1966,7 +1970,7 @@
       <c r="E51" t="s">
         <v>11</v>
       </c>
-      <c r="F51" s="2" t="s">
+      <c r="F51" s="1" t="s">
         <v>64</v>
       </c>
       <c r="G51">
@@ -1975,7 +1979,7 @@
       <c r="H51">
         <v>0</v>
       </c>
-      <c r="I51" s="1">
+      <c r="I51" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -1995,10 +1999,10 @@
       <c r="E52" t="s">
         <v>13</v>
       </c>
-      <c r="F52" s="2" t="s">
+      <c r="F52" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="I52" s="1">
+      <c r="I52" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -2018,7 +2022,7 @@
       <c r="E53" t="s">
         <v>13</v>
       </c>
-      <c r="F53" s="2" t="s">
+      <c r="F53" s="1" t="s">
         <v>66</v>
       </c>
       <c r="G53">
@@ -2027,7 +2031,7 @@
       <c r="H53">
         <v>0</v>
       </c>
-      <c r="I53" s="1">
+      <c r="I53" s="3">
         <v>41820</v>
       </c>
     </row>
@@ -2047,8 +2051,11 @@
       <c r="E54" t="s">
         <v>13</v>
       </c>
-      <c r="G54" s="3">
+      <c r="G54" s="2">
         <v>41.6</v>
+      </c>
+      <c r="I54" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2067,8 +2074,11 @@
       <c r="E55" t="s">
         <v>11</v>
       </c>
-      <c r="G55" s="3">
+      <c r="G55" s="2">
         <v>41</v>
+      </c>
+      <c r="I55" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="56" spans="1:9">
@@ -2087,8 +2097,11 @@
       <c r="E56" t="s">
         <v>13</v>
       </c>
-      <c r="G56" s="3">
+      <c r="G56" s="2">
         <v>41</v>
+      </c>
+      <c r="I56" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="57" spans="1:9">
@@ -2107,8 +2120,14 @@
       <c r="E57" t="s">
         <v>13</v>
       </c>
-      <c r="G57" s="3">
+      <c r="G57" s="2">
         <v>41.2</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="58" spans="1:9">
@@ -2127,8 +2146,11 @@
       <c r="E58" t="s">
         <v>11</v>
       </c>
-      <c r="G58" s="3">
+      <c r="G58" s="2">
         <v>39.799999999999997</v>
+      </c>
+      <c r="I58" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="59" spans="1:9">
@@ -2147,8 +2169,11 @@
       <c r="E59" t="s">
         <v>11</v>
       </c>
-      <c r="G59" s="3">
+      <c r="G59" s="2">
         <v>41.6</v>
+      </c>
+      <c r="I59" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="60" spans="1:9">
@@ -2167,8 +2192,11 @@
       <c r="E60" t="s">
         <v>11</v>
       </c>
-      <c r="G60" s="3">
+      <c r="G60" s="2">
         <v>41</v>
+      </c>
+      <c r="I60" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="61" spans="1:9">
@@ -2187,8 +2215,11 @@
       <c r="E61" t="s">
         <v>11</v>
       </c>
-      <c r="G61" s="3">
+      <c r="G61" s="2">
         <v>39</v>
+      </c>
+      <c r="I61" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="62" spans="1:9">
@@ -2207,8 +2238,11 @@
       <c r="E62" t="s">
         <v>13</v>
       </c>
-      <c r="G62" s="3">
+      <c r="G62" s="2">
         <v>41</v>
+      </c>
+      <c r="I62" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="63" spans="1:9">
@@ -2227,8 +2261,11 @@
       <c r="E63" t="s">
         <v>11</v>
       </c>
-      <c r="G63" s="3">
+      <c r="G63" s="2">
         <v>41.6</v>
+      </c>
+      <c r="I63" s="3">
+        <v>41821</v>
       </c>
     </row>
     <row r="64" spans="1:9">
@@ -2247,11 +2284,14 @@
       <c r="E64" t="s">
         <v>11</v>
       </c>
-      <c r="G64" s="3">
+      <c r="G64" s="2">
         <v>41</v>
       </c>
-    </row>
-    <row r="65" spans="1:7">
+      <c r="I64" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2267,11 +2307,14 @@
       <c r="E65" t="s">
         <v>11</v>
       </c>
-      <c r="G65" s="3">
+      <c r="G65" s="2">
         <v>40.4</v>
       </c>
-    </row>
-    <row r="66" spans="1:7">
+      <c r="I65" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2287,11 +2330,14 @@
       <c r="E66" t="s">
         <v>13</v>
       </c>
-      <c r="G66" s="3">
+      <c r="G66" s="2">
         <v>37.1</v>
       </c>
-    </row>
-    <row r="67" spans="1:7">
+      <c r="I66" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
       <c r="A67">
         <v>2</v>
       </c>
@@ -2307,11 +2353,14 @@
       <c r="E67" t="s">
         <v>13</v>
       </c>
-      <c r="F67" s="2" t="s">
+      <c r="F67" s="1" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="68" spans="1:7">
+      <c r="I67" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9">
       <c r="A68">
         <v>2</v>
       </c>
@@ -2327,11 +2376,14 @@
       <c r="E68" t="s">
         <v>13</v>
       </c>
-      <c r="F68" s="2" t="s">
+      <c r="F68" s="1" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="69" spans="1:7">
+      <c r="I68" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9">
       <c r="A69">
         <v>2</v>
       </c>
@@ -2347,11 +2399,14 @@
       <c r="E69" t="s">
         <v>11</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F69" s="1" t="s">
         <v>74</v>
       </c>
-    </row>
-    <row r="70" spans="1:7">
+      <c r="I69" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9">
       <c r="A70">
         <v>2</v>
       </c>
@@ -2367,11 +2422,14 @@
       <c r="E70" t="s">
         <v>11</v>
       </c>
-      <c r="F70" s="2" t="s">
+      <c r="F70" s="1" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="71" spans="1:7">
+      <c r="I70" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9">
       <c r="A71">
         <v>2</v>
       </c>
@@ -2387,11 +2445,14 @@
       <c r="E71" t="s">
         <v>13</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F71" s="1" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="72" spans="1:7">
+      <c r="I71" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9">
       <c r="A72">
         <v>2</v>
       </c>
@@ -2407,11 +2468,14 @@
       <c r="E72" t="s">
         <v>13</v>
       </c>
-      <c r="F72" s="2" t="s">
+      <c r="F72" s="1" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="73" spans="1:7">
+      <c r="I72" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9">
       <c r="A73">
         <v>2</v>
       </c>
@@ -2427,11 +2491,14 @@
       <c r="E73" t="s">
         <v>13</v>
       </c>
-      <c r="F73" s="2" t="s">
+      <c r="F73" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="74" spans="1:7">
+      <c r="I73" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9">
       <c r="A74">
         <v>2</v>
       </c>
@@ -2447,11 +2514,14 @@
       <c r="E74" t="s">
         <v>13</v>
       </c>
-      <c r="F74" s="2" t="s">
+      <c r="F74" s="1" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="75" spans="1:7">
+      <c r="I74" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9">
       <c r="A75">
         <v>2</v>
       </c>
@@ -2467,11 +2537,14 @@
       <c r="E75" t="s">
         <v>11</v>
       </c>
-      <c r="F75" s="2" t="s">
+      <c r="F75" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="76" spans="1:7">
+      <c r="I75" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9">
       <c r="A76">
         <v>2</v>
       </c>
@@ -2487,11 +2560,14 @@
       <c r="E76" t="s">
         <v>13</v>
       </c>
-      <c r="F76" s="2" t="s">
+      <c r="F76" s="1" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="77" spans="1:7">
+      <c r="I76" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9">
       <c r="A77">
         <v>2</v>
       </c>
@@ -2507,11 +2583,17 @@
       <c r="E77" t="s">
         <v>13</v>
       </c>
-      <c r="F77" s="2" t="s">
+      <c r="F77" s="1" t="s">
         <v>82</v>
       </c>
-    </row>
-    <row r="78" spans="1:7">
+      <c r="H77">
+        <v>0</v>
+      </c>
+      <c r="I77" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9">
       <c r="A78">
         <v>2</v>
       </c>
@@ -2527,11 +2609,14 @@
       <c r="E78" t="s">
         <v>13</v>
       </c>
-      <c r="F78" s="2" t="s">
+      <c r="F78" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="79" spans="1:7">
+      <c r="I78" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9">
       <c r="A79">
         <v>2</v>
       </c>
@@ -2547,11 +2632,14 @@
       <c r="E79" t="s">
         <v>11</v>
       </c>
-      <c r="F79" s="2" t="s">
+      <c r="F79" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="80" spans="1:7">
+      <c r="I79" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9">
       <c r="A80">
         <v>2</v>
       </c>
@@ -2567,11 +2655,14 @@
       <c r="E80" t="s">
         <v>11</v>
       </c>
-      <c r="F80" s="2" t="s">
+      <c r="F80" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="81" spans="1:7">
+      <c r="I80" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9">
       <c r="A81">
         <v>2</v>
       </c>
@@ -2587,11 +2678,17 @@
       <c r="E81" t="s">
         <v>13</v>
       </c>
-      <c r="F81" s="2" t="s">
+      <c r="F81" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="82" spans="1:7">
+      <c r="H81">
+        <v>0</v>
+      </c>
+      <c r="I81" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9">
       <c r="A82">
         <v>2</v>
       </c>
@@ -2607,11 +2704,17 @@
       <c r="E82" t="s">
         <v>13</v>
       </c>
-      <c r="F82" s="2" t="s">
+      <c r="F82" s="1" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="83" spans="1:7">
+      <c r="H82">
+        <v>0</v>
+      </c>
+      <c r="I82" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9">
       <c r="A83">
         <v>2</v>
       </c>
@@ -2627,11 +2730,17 @@
       <c r="E83" t="s">
         <v>11</v>
       </c>
-      <c r="F83" s="2" t="s">
+      <c r="F83" s="1" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="84" spans="1:7">
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9">
       <c r="A84">
         <v>2</v>
       </c>
@@ -2647,11 +2756,14 @@
       <c r="E84" t="s">
         <v>13</v>
       </c>
-      <c r="F84" s="2" t="s">
+      <c r="F84" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="85" spans="1:7">
+      <c r="I84" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9">
       <c r="A85">
         <v>2</v>
       </c>
@@ -2667,11 +2779,14 @@
       <c r="E85" t="s">
         <v>13</v>
       </c>
-      <c r="F85" s="2" t="s">
+      <c r="F85" s="1" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="86" spans="1:7">
+      <c r="I85" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9">
       <c r="A86">
         <v>2</v>
       </c>
@@ -2687,11 +2802,14 @@
       <c r="E86" t="s">
         <v>13</v>
       </c>
-      <c r="F86" s="2" t="s">
+      <c r="F86" s="1" t="s">
         <v>91</v>
       </c>
-    </row>
-    <row r="87" spans="1:7">
+      <c r="I86" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9">
       <c r="A87">
         <v>2</v>
       </c>
@@ -2707,11 +2825,14 @@
       <c r="E87" t="s">
         <v>11</v>
       </c>
-      <c r="F87" s="2" t="s">
+      <c r="F87" s="1" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="88" spans="1:7">
+      <c r="I87" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9">
       <c r="A88">
         <v>2</v>
       </c>
@@ -2727,11 +2848,14 @@
       <c r="E88" t="s">
         <v>11</v>
       </c>
-      <c r="F88" s="2" t="s">
+      <c r="F88" s="1" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="89" spans="1:7">
+      <c r="I88" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9">
       <c r="A89">
         <v>2</v>
       </c>
@@ -2747,11 +2871,14 @@
       <c r="E89" t="s">
         <v>13</v>
       </c>
-      <c r="F89" s="2" t="s">
+      <c r="F89" s="1" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="90" spans="1:7">
+      <c r="I89" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9">
       <c r="A90">
         <v>2</v>
       </c>
@@ -2767,11 +2894,17 @@
       <c r="E90" t="s">
         <v>13</v>
       </c>
-      <c r="F90" s="2" t="s">
+      <c r="F90" s="1" t="s">
         <v>95</v>
       </c>
-    </row>
-    <row r="91" spans="1:7">
+      <c r="H90">
+        <v>0</v>
+      </c>
+      <c r="I90" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9">
       <c r="A91">
         <v>2</v>
       </c>
@@ -2787,11 +2920,14 @@
       <c r="E91" t="s">
         <v>13</v>
       </c>
-      <c r="F91" s="2" t="s">
+      <c r="F91" s="1" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="92" spans="1:7">
+      <c r="I91" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
       <c r="A92">
         <v>2</v>
       </c>
@@ -2807,11 +2943,14 @@
       <c r="E92" t="s">
         <v>13</v>
       </c>
-      <c r="F92" s="2" t="s">
+      <c r="F92" s="1" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="93" spans="1:7">
+      <c r="I92" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
       <c r="A93">
         <v>2</v>
       </c>
@@ -2830,8 +2969,14 @@
       <c r="G93">
         <v>39.299999999999997</v>
       </c>
-    </row>
-    <row r="94" spans="1:7">
+      <c r="H93">
+        <v>0</v>
+      </c>
+      <c r="I93" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
       <c r="A94">
         <v>2</v>
       </c>
@@ -2850,8 +2995,11 @@
       <c r="G94">
         <v>38.1</v>
       </c>
-    </row>
-    <row r="95" spans="1:7">
+      <c r="I94" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
       <c r="A95">
         <v>2</v>
       </c>
@@ -2870,8 +3018,14 @@
       <c r="G95">
         <v>38.9</v>
       </c>
-    </row>
-    <row r="96" spans="1:7">
+      <c r="H95">
+        <v>0</v>
+      </c>
+      <c r="I95" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
       <c r="A96">
         <v>2</v>
       </c>
@@ -2890,8 +3044,11 @@
       <c r="G96">
         <v>39</v>
       </c>
-    </row>
-    <row r="97" spans="1:7">
+      <c r="I96" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
       <c r="A97">
         <v>2</v>
       </c>
@@ -2910,8 +3067,11 @@
       <c r="G97">
         <v>37.6</v>
       </c>
-    </row>
-    <row r="98" spans="1:7">
+      <c r="I97" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
       <c r="A98">
         <v>2</v>
       </c>
@@ -2930,8 +3090,11 @@
       <c r="G98">
         <v>39.5</v>
       </c>
-    </row>
-    <row r="99" spans="1:7">
+      <c r="I98" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
       <c r="A99">
         <v>2</v>
       </c>
@@ -2950,8 +3113,11 @@
       <c r="G99">
         <v>37.200000000000003</v>
       </c>
-    </row>
-    <row r="100" spans="1:7">
+      <c r="I99" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
       <c r="A100">
         <v>2</v>
       </c>
@@ -2970,8 +3136,11 @@
       <c r="G100">
         <v>38.700000000000003</v>
       </c>
-    </row>
-    <row r="101" spans="1:7">
+      <c r="I100" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
       <c r="A101">
         <v>2</v>
       </c>
@@ -2990,8 +3159,11 @@
       <c r="G101">
         <v>39.4</v>
       </c>
-    </row>
-    <row r="102" spans="1:7">
+      <c r="I101" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
       <c r="A102">
         <v>2</v>
       </c>
@@ -3010,8 +3182,11 @@
       <c r="G102">
         <v>37.1</v>
       </c>
-    </row>
-    <row r="103" spans="1:7">
+      <c r="I102" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
       <c r="A103">
         <v>2</v>
       </c>
@@ -3030,8 +3205,11 @@
       <c r="G103">
         <v>39.1</v>
       </c>
-    </row>
-    <row r="104" spans="1:7">
+      <c r="I103" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
       <c r="A104">
         <v>2</v>
       </c>
@@ -3050,8 +3228,11 @@
       <c r="G104">
         <v>37</v>
       </c>
-    </row>
-    <row r="105" spans="1:7">
+      <c r="I104" s="3">
+        <v>41821</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
       <c r="A105">
         <v>2</v>
       </c>
@@ -3068,7 +3249,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="106" spans="1:7">
+    <row r="106" spans="1:9">
       <c r="A106">
         <v>3</v>
       </c>
@@ -3085,7 +3266,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="107" spans="1:7">
+    <row r="107" spans="1:9">
       <c r="A107">
         <v>3</v>
       </c>
@@ -3102,7 +3283,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="108" spans="1:7">
+    <row r="108" spans="1:9">
       <c r="A108">
         <v>3</v>
       </c>
@@ -3119,7 +3300,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="109" spans="1:7">
+    <row r="109" spans="1:9">
       <c r="A109">
         <v>3</v>
       </c>
@@ -3136,7 +3317,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="110" spans="1:7">
+    <row r="110" spans="1:9">
       <c r="A110">
         <v>3</v>
       </c>
@@ -3153,7 +3334,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="111" spans="1:7">
+    <row r="111" spans="1:9">
       <c r="A111">
         <v>3</v>
       </c>
@@ -3170,7 +3351,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="112" spans="1:7">
+    <row r="112" spans="1:9">
       <c r="A112">
         <v>3</v>
       </c>

</xml_diff>